<commit_message>
fixed small error in rule for lastfollowup valid.warning rule
</commit_message>
<xml_diff>
--- a/BCRPP_QC_R_Excel_Program/Core QC Rules/BCRPP Warning Rules.xlsx
+++ b/BCRPP_QC_R_Excel_Program/Core QC Rules/BCRPP Warning Rules.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11028"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D778C6-814F-8C45-911D-E1BCCDA260FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC147AC-4B5E-974E-9ECB-0A36DBC4CA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1091,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T39" sqref="T39"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1350,7 +1350,7 @@
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>44</v>
       </c>
       <c r="S9" s="2" t="s">

</xml_diff>